<commit_message>
add bdd cucumber part 1
</commit_message>
<xml_diff>
--- a/wedemy-failed.xlsx
+++ b/wedemy-failed.xlsx
@@ -1,31 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imam-pc\Katalon Studio\katalon-test1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1943DDA3-F107-4E0B-91B4-DC19B8AD62E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="20490" windowHeight="7080" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
+    <sheet name="profile" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>username</t>
   </si>
@@ -35,29 +25,375 @@
   <si>
     <t>studentx</t>
   </si>
+  <si>
+    <t>id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -65,24 +401,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -131,7 +753,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -166,7 +788,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -206,7 +828,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -230,9 +852,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -256,7 +878,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -309,7 +931,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -334,35 +956,30 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85833333333333" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -380,5 +997,33 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>11111</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change data excel cell in json format
</commit_message>
<xml_diff>
--- a/wedemy-failed.xlsx
+++ b/wedemy-failed.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imam-pc\Katalon Studio\katalon-test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F2A10AB-0DAD-40F4-86FC-CE01138F0C45}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1B0366-895E-4553-9C1E-2961D1BD8701}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login admin" sheetId="1" r:id="rId1"/>
@@ -22,42 +22,65 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="8">
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>pass</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>adminx</t>
-  </si>
-  <si>
-    <t>admin01</t>
-  </si>
-  <si>
-    <t>salah</t>
-  </si>
-  <si>
-    <t>student</t>
-  </si>
-  <si>
-    <t>stundent1</t>
+    <t>data</t>
+  </si>
+  <si>
+    <t>{
+  "username" : "salah",
+  "userPassword" : "12345678"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "username" : "admin01",
+  "userPassword" : "salah"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "username" : "salah",
+  "userPassword" : "salah"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "username" : "salah"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "userPassword" : "salah"
+}</t>
+  </si>
+  <si>
+    <t>{
+  "username" : student",
+  "userPassword" : "salah"
+}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -81,8 +104,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,68 +387,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="60">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="60">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:1" ht="60">
+      <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:1" ht="45">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="B4">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>5</v>
+    <row r="6" spans="1:1" ht="45">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -429,64 +436,45 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB564929-B027-45CF-9430-6EB106CBC3DB}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:1">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="60">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="60">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    </row>
+    <row r="4" spans="1:1" ht="60">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="45">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="45">
+      <c r="A6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="B4">
-        <v>12345678</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -506,7 +494,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">

</xml_diff>